<commit_message>
excel basic 11 v-2
</commit_message>
<xml_diff>
--- a/excelBasic11Formula.xlsx
+++ b/excelBasic11Formula.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github Public Repo\Excel-Formula-Note\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC99E1B-7E99-4146-8E4C-404F4FB33957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9B534D-4C15-4A20-BFB7-6EBE82629579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>SL</t>
   </si>
@@ -80,6 +80,21 @@
   </si>
   <si>
     <t>Upto Total</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>CountA</t>
+  </si>
+  <si>
+    <t>CountIF</t>
   </si>
 </sst>
 </file>
@@ -116,12 +131,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -153,11 +174,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -177,6 +195,11 @@
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,37 +482,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -512,230 +552,258 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>38181</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7">
+      <c r="D3" s="5"/>
+      <c r="E3" s="6">
         <f>C3+D3</f>
         <v>38181</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>751017</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>8546</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="7">
         <f>F3+G3</f>
         <v>759563</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K3" s="7">
+        <f>SUM(C3:H3)</f>
+        <v>1595488</v>
+      </c>
+      <c r="L3" s="7">
+        <f>AVERAGE(C3:H3)</f>
+        <v>319097.59999999998</v>
+      </c>
+      <c r="M3">
+        <f>COUNT(A3:H3)</f>
+        <v>6</v>
+      </c>
+      <c r="N3">
+        <f>COUNTA(A3:H3)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>18406</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="7">
+      <c r="D4" s="4"/>
+      <c r="E4" s="6">
         <f t="shared" ref="E4:E8" si="0">C4+D4</f>
         <v>18406</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>644597</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>16561</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="7">
         <f t="shared" ref="H4:H8" si="1">F4+G4</f>
         <v>661158</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K4" s="9">
+        <f>SUM(C4:E4,E6:H6)</f>
+        <v>936918</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>8932</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="7">
+      <c r="D5" s="4"/>
+      <c r="E5" s="6">
         <f t="shared" si="0"/>
         <v>8932</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>535737</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="8">
+      <c r="G5" s="1"/>
+      <c r="H5" s="7">
         <f t="shared" si="1"/>
         <v>535737</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K5" s="10">
+        <f>SUM(C5+D5+E5+F5+G5+H5)</f>
+        <v>1089338</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>10402</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="7">
+      <c r="D6" s="4"/>
+      <c r="E6" s="6">
         <f t="shared" si="0"/>
         <v>10402</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>444852</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="8">
+      <c r="G6" s="1"/>
+      <c r="H6" s="7">
         <f t="shared" si="1"/>
         <v>444852</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K6" s="7">
+        <f>SUM(C6,D6,E6,F6,G6,H6)</f>
+        <v>910508</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>102564</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="7">
+      <c r="D7" s="4"/>
+      <c r="E7" s="6">
         <f t="shared" si="0"/>
         <v>102564</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>2924553</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>25107</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="7">
         <f t="shared" si="1"/>
         <v>2949660</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>10278</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="7">
+      <c r="D8" s="4"/>
+      <c r="E8" s="6">
         <f t="shared" si="0"/>
         <v>10278</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>400410</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>80511</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <f t="shared" si="1"/>
         <v>480921</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>38181</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7">
+      <c r="D9" s="5"/>
+      <c r="E9" s="6">
         <f>C9+D9</f>
         <v>38181</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>751017</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>8546</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <f>F9+G9</f>
         <v>759563</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>18406</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="7">
+      <c r="D10" s="4"/>
+      <c r="E10" s="6">
         <f t="shared" ref="E10:E11" si="2">C10+D10</f>
         <v>18406</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>644597</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>16561</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="7">
         <f t="shared" ref="H10:H11" si="3">F10+G10</f>
         <v>661158</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>8932</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="7">
+      <c r="D11" s="4"/>
+      <c r="E11" s="6">
         <f t="shared" si="2"/>
         <v>8932</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>535737</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="8">
+      <c r="G11" s="1"/>
+      <c r="H11" s="7">
         <f t="shared" si="3"/>
         <v>535737</v>
       </c>

</xml_diff>